<commit_message>
Creata connessione al db
</commit_message>
<xml_diff>
--- a/upload/CDR-ERICSSON-MSRBS-SU_FG53RNC_Rev.6 (1).xlsx
+++ b/upload/CDR-ERICSSON-MSRBS-SU_FG53RNC_Rev.6 (1).xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITadmin\Desktop\Ericsson\CDR trasport\FG53RNC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\autoupdate\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4362,17 +4362,35 @@
     <xf numFmtId="0" fontId="54" fillId="39" borderId="39" xfId="167" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="40" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="40" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="35" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="28" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="28" borderId="3" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="34" borderId="33" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="34" borderId="34" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="29" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4392,16 +4410,7 @@
     <xf numFmtId="0" fontId="49" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="28" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="28" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4470,32 +4479,23 @@
     <xf numFmtId="0" fontId="49" fillId="27" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="40" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="40" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="28" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="35" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="28" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="35" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="28" borderId="3" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="34" borderId="33" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="34" borderId="34" xfId="112" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5164,8 +5164,8 @@
   </sheetPr>
   <dimension ref="A1:CF35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CC19" sqref="CC19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5237,339 +5237,339 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:84" ht="15" customHeight="1">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145" t="s">
+      <c r="B1" s="109" t="s">
         <v>237</v>
       </c>
-      <c r="C1" s="152" t="s">
+      <c r="C1" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="123" t="s">
+      <c r="D1" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="129" t="s">
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
-      <c r="L1" s="130"/>
-      <c r="M1" s="130"/>
-      <c r="N1" s="130"/>
-      <c r="O1" s="130"/>
-      <c r="P1" s="130"/>
-      <c r="Q1" s="130"/>
-      <c r="R1" s="130"/>
-      <c r="S1" s="130"/>
-      <c r="T1" s="130"/>
-      <c r="U1" s="130"/>
-      <c r="V1" s="131"/>
-      <c r="W1" s="135" t="s">
+      <c r="J1" s="133"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
+      <c r="O1" s="133"/>
+      <c r="P1" s="133"/>
+      <c r="Q1" s="133"/>
+      <c r="R1" s="133"/>
+      <c r="S1" s="133"/>
+      <c r="T1" s="133"/>
+      <c r="U1" s="133"/>
+      <c r="V1" s="134"/>
+      <c r="W1" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="136"/>
-      <c r="Y1" s="136"/>
-      <c r="Z1" s="136"/>
-      <c r="AA1" s="137"/>
-      <c r="AB1" s="113" t="s">
+      <c r="X1" s="139"/>
+      <c r="Y1" s="139"/>
+      <c r="Z1" s="139"/>
+      <c r="AA1" s="140"/>
+      <c r="AB1" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="AC1" s="114"/>
-      <c r="AD1" s="114"/>
-      <c r="AE1" s="114"/>
-      <c r="AF1" s="114"/>
-      <c r="AG1" s="114"/>
-      <c r="AH1" s="115"/>
-      <c r="AI1" s="113" t="s">
+      <c r="AC1" s="120"/>
+      <c r="AD1" s="120"/>
+      <c r="AE1" s="120"/>
+      <c r="AF1" s="120"/>
+      <c r="AG1" s="120"/>
+      <c r="AH1" s="121"/>
+      <c r="AI1" s="119" t="s">
         <v>195</v>
       </c>
-      <c r="AJ1" s="114"/>
-      <c r="AK1" s="114"/>
-      <c r="AL1" s="114"/>
-      <c r="AM1" s="114"/>
-      <c r="AN1" s="114"/>
-      <c r="AO1" s="115"/>
-      <c r="AP1" s="119" t="s">
+      <c r="AJ1" s="120"/>
+      <c r="AK1" s="120"/>
+      <c r="AL1" s="120"/>
+      <c r="AM1" s="120"/>
+      <c r="AN1" s="120"/>
+      <c r="AO1" s="121"/>
+      <c r="AP1" s="150" t="s">
         <v>17</v>
       </c>
-      <c r="AQ1" s="120"/>
-      <c r="AR1" s="120"/>
-      <c r="AS1" s="120"/>
-      <c r="AT1" s="120"/>
-      <c r="AU1" s="120"/>
-      <c r="AV1" s="120"/>
-      <c r="AW1" s="120"/>
-      <c r="AX1" s="120"/>
-      <c r="AY1" s="120"/>
-      <c r="AZ1" s="120"/>
-      <c r="BA1" s="120"/>
-      <c r="BB1" s="120"/>
-      <c r="BC1" s="120"/>
-      <c r="BD1" s="120"/>
-      <c r="BE1" s="120"/>
-      <c r="BF1" s="120"/>
-      <c r="BG1" s="120"/>
-      <c r="BH1" s="120"/>
-      <c r="BI1" s="120"/>
-      <c r="BJ1" s="120"/>
-      <c r="BK1" s="120"/>
-      <c r="BL1" s="120"/>
-      <c r="BM1" s="120"/>
-      <c r="BN1" s="120"/>
-      <c r="BO1" s="120"/>
-      <c r="BP1" s="120"/>
-      <c r="BQ1" s="120"/>
-      <c r="BR1" s="120"/>
-      <c r="BS1" s="120"/>
-      <c r="BT1" s="120"/>
-      <c r="BU1" s="120"/>
-      <c r="BV1" s="120"/>
-      <c r="BW1" s="120"/>
-      <c r="BX1" s="121"/>
-      <c r="BY1" s="121"/>
-      <c r="BZ1" s="121"/>
-      <c r="CA1" s="121"/>
-      <c r="CB1" s="121"/>
-      <c r="CC1" s="122"/>
-      <c r="CD1" s="148" t="s">
+      <c r="AQ1" s="151"/>
+      <c r="AR1" s="151"/>
+      <c r="AS1" s="151"/>
+      <c r="AT1" s="151"/>
+      <c r="AU1" s="151"/>
+      <c r="AV1" s="151"/>
+      <c r="AW1" s="151"/>
+      <c r="AX1" s="151"/>
+      <c r="AY1" s="151"/>
+      <c r="AZ1" s="151"/>
+      <c r="BA1" s="151"/>
+      <c r="BB1" s="151"/>
+      <c r="BC1" s="151"/>
+      <c r="BD1" s="151"/>
+      <c r="BE1" s="151"/>
+      <c r="BF1" s="151"/>
+      <c r="BG1" s="151"/>
+      <c r="BH1" s="151"/>
+      <c r="BI1" s="151"/>
+      <c r="BJ1" s="151"/>
+      <c r="BK1" s="151"/>
+      <c r="BL1" s="151"/>
+      <c r="BM1" s="151"/>
+      <c r="BN1" s="151"/>
+      <c r="BO1" s="151"/>
+      <c r="BP1" s="151"/>
+      <c r="BQ1" s="151"/>
+      <c r="BR1" s="151"/>
+      <c r="BS1" s="151"/>
+      <c r="BT1" s="151"/>
+      <c r="BU1" s="151"/>
+      <c r="BV1" s="151"/>
+      <c r="BW1" s="151"/>
+      <c r="BX1" s="152"/>
+      <c r="BY1" s="152"/>
+      <c r="BZ1" s="152"/>
+      <c r="CA1" s="152"/>
+      <c r="CB1" s="152"/>
+      <c r="CC1" s="153"/>
+      <c r="CD1" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="CE1" s="109" t="s">
+      <c r="CE1" s="148" t="s">
         <v>256</v>
       </c>
-      <c r="CF1" s="110"/>
+      <c r="CF1" s="149"/>
     </row>
     <row r="2" spans="1:84" ht="15" customHeight="1">
-      <c r="A2" s="146"/>
-      <c r="B2" s="146"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="132"/>
-      <c r="J2" s="133"/>
-      <c r="K2" s="133"/>
-      <c r="L2" s="133"/>
-      <c r="M2" s="133"/>
-      <c r="N2" s="133"/>
-      <c r="O2" s="133"/>
-      <c r="P2" s="133"/>
-      <c r="Q2" s="133"/>
-      <c r="R2" s="133"/>
-      <c r="S2" s="133"/>
-      <c r="T2" s="133"/>
-      <c r="U2" s="133"/>
-      <c r="V2" s="134"/>
-      <c r="W2" s="138"/>
-      <c r="X2" s="139"/>
-      <c r="Y2" s="139"/>
-      <c r="Z2" s="139"/>
-      <c r="AA2" s="140"/>
-      <c r="AB2" s="116"/>
-      <c r="AC2" s="117"/>
-      <c r="AD2" s="117"/>
-      <c r="AE2" s="117"/>
-      <c r="AF2" s="117"/>
-      <c r="AG2" s="117"/>
-      <c r="AH2" s="118"/>
-      <c r="AI2" s="116"/>
-      <c r="AJ2" s="117"/>
-      <c r="AK2" s="117"/>
-      <c r="AL2" s="117"/>
-      <c r="AM2" s="117"/>
-      <c r="AN2" s="117"/>
-      <c r="AO2" s="118"/>
-      <c r="AP2" s="150" t="s">
+      <c r="A2" s="110"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="130"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="136"/>
+      <c r="M2" s="136"/>
+      <c r="N2" s="136"/>
+      <c r="O2" s="136"/>
+      <c r="P2" s="136"/>
+      <c r="Q2" s="136"/>
+      <c r="R2" s="136"/>
+      <c r="S2" s="136"/>
+      <c r="T2" s="136"/>
+      <c r="U2" s="136"/>
+      <c r="V2" s="137"/>
+      <c r="W2" s="141"/>
+      <c r="X2" s="142"/>
+      <c r="Y2" s="142"/>
+      <c r="Z2" s="142"/>
+      <c r="AA2" s="143"/>
+      <c r="AB2" s="122"/>
+      <c r="AC2" s="123"/>
+      <c r="AD2" s="123"/>
+      <c r="AE2" s="123"/>
+      <c r="AF2" s="123"/>
+      <c r="AG2" s="123"/>
+      <c r="AH2" s="124"/>
+      <c r="AI2" s="122"/>
+      <c r="AJ2" s="123"/>
+      <c r="AK2" s="123"/>
+      <c r="AL2" s="123"/>
+      <c r="AM2" s="123"/>
+      <c r="AN2" s="123"/>
+      <c r="AO2" s="124"/>
+      <c r="AP2" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="AQ2" s="111" t="s">
+      <c r="AQ2" s="115" t="s">
         <v>32</v>
       </c>
-      <c r="AR2" s="111"/>
-      <c r="AS2" s="111"/>
-      <c r="AT2" s="111"/>
-      <c r="AU2" s="111"/>
-      <c r="AV2" s="111"/>
-      <c r="AW2" s="111" t="s">
+      <c r="AR2" s="115"/>
+      <c r="AS2" s="115"/>
+      <c r="AT2" s="115"/>
+      <c r="AU2" s="115"/>
+      <c r="AV2" s="115"/>
+      <c r="AW2" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="AX2" s="111"/>
-      <c r="AY2" s="111"/>
-      <c r="AZ2" s="111" t="s">
+      <c r="AX2" s="115"/>
+      <c r="AY2" s="115"/>
+      <c r="AZ2" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="BA2" s="111"/>
-      <c r="BB2" s="111"/>
-      <c r="BC2" s="111" t="s">
+      <c r="BA2" s="115"/>
+      <c r="BB2" s="115"/>
+      <c r="BC2" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="BD2" s="111"/>
-      <c r="BE2" s="111"/>
-      <c r="BF2" s="111" t="s">
+      <c r="BD2" s="115"/>
+      <c r="BE2" s="115"/>
+      <c r="BF2" s="115" t="s">
         <v>55</v>
       </c>
-      <c r="BG2" s="111"/>
-      <c r="BH2" s="111"/>
-      <c r="BI2" s="111" t="s">
+      <c r="BG2" s="115"/>
+      <c r="BH2" s="115"/>
+      <c r="BI2" s="115" t="s">
         <v>56</v>
       </c>
-      <c r="BJ2" s="111"/>
-      <c r="BK2" s="111"/>
-      <c r="BL2" s="111" t="s">
+      <c r="BJ2" s="115"/>
+      <c r="BK2" s="115"/>
+      <c r="BL2" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="BM2" s="111"/>
-      <c r="BN2" s="111"/>
-      <c r="BO2" s="111" t="s">
+      <c r="BM2" s="115"/>
+      <c r="BN2" s="115"/>
+      <c r="BO2" s="115" t="s">
         <v>58</v>
       </c>
-      <c r="BP2" s="111"/>
-      <c r="BQ2" s="111"/>
-      <c r="BR2" s="111" t="s">
+      <c r="BP2" s="115"/>
+      <c r="BQ2" s="115"/>
+      <c r="BR2" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="BS2" s="111"/>
-      <c r="BT2" s="111"/>
-      <c r="BU2" s="111" t="s">
+      <c r="BS2" s="115"/>
+      <c r="BT2" s="115"/>
+      <c r="BU2" s="115" t="s">
         <v>29</v>
       </c>
-      <c r="BV2" s="111"/>
-      <c r="BW2" s="112"/>
-      <c r="BX2" s="111" t="s">
+      <c r="BV2" s="115"/>
+      <c r="BW2" s="125"/>
+      <c r="BX2" s="115" t="s">
         <v>208</v>
       </c>
-      <c r="BY2" s="111"/>
-      <c r="BZ2" s="112"/>
-      <c r="CA2" s="111" t="s">
+      <c r="BY2" s="115"/>
+      <c r="BZ2" s="125"/>
+      <c r="CA2" s="115" t="s">
         <v>215</v>
       </c>
-      <c r="CB2" s="111"/>
-      <c r="CC2" s="112"/>
-      <c r="CD2" s="149"/>
-      <c r="CE2" s="109"/>
-      <c r="CF2" s="110"/>
+      <c r="CB2" s="115"/>
+      <c r="CC2" s="125"/>
+      <c r="CD2" s="113"/>
+      <c r="CE2" s="148"/>
+      <c r="CF2" s="149"/>
     </row>
     <row r="3" spans="1:84" ht="15" customHeight="1">
-      <c r="A3" s="146"/>
-      <c r="B3" s="146"/>
-      <c r="C3" s="153"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="141" t="s">
+      <c r="A3" s="110"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="142" t="s">
+      <c r="J3" s="145" t="s">
         <v>68</v>
       </c>
-      <c r="K3" s="133"/>
-      <c r="L3" s="133"/>
-      <c r="M3" s="142" t="s">
+      <c r="K3" s="136"/>
+      <c r="L3" s="136"/>
+      <c r="M3" s="145" t="s">
         <v>69</v>
       </c>
-      <c r="N3" s="133"/>
-      <c r="O3" s="133"/>
-      <c r="P3" s="142" t="s">
+      <c r="N3" s="136"/>
+      <c r="O3" s="136"/>
+      <c r="P3" s="145" t="s">
         <v>70</v>
       </c>
-      <c r="Q3" s="133"/>
-      <c r="R3" s="133"/>
-      <c r="S3" s="142" t="s">
+      <c r="Q3" s="136"/>
+      <c r="R3" s="136"/>
+      <c r="S3" s="145" t="s">
         <v>11</v>
       </c>
-      <c r="T3" s="144" t="s">
+      <c r="T3" s="147" t="s">
         <v>77</v>
       </c>
-      <c r="U3" s="144" t="s">
+      <c r="U3" s="147" t="s">
         <v>79</v>
       </c>
-      <c r="V3" s="143" t="s">
+      <c r="V3" s="146" t="s">
         <v>30</v>
       </c>
-      <c r="W3" s="138"/>
-      <c r="X3" s="139"/>
-      <c r="Y3" s="139"/>
-      <c r="Z3" s="139"/>
-      <c r="AA3" s="140"/>
-      <c r="AB3" s="116"/>
-      <c r="AC3" s="117"/>
-      <c r="AD3" s="117"/>
-      <c r="AE3" s="117"/>
-      <c r="AF3" s="117"/>
-      <c r="AG3" s="117"/>
-      <c r="AH3" s="118"/>
-      <c r="AI3" s="116"/>
-      <c r="AJ3" s="117"/>
-      <c r="AK3" s="117"/>
-      <c r="AL3" s="117"/>
-      <c r="AM3" s="117"/>
-      <c r="AN3" s="117"/>
-      <c r="AO3" s="118"/>
-      <c r="AP3" s="150"/>
+      <c r="W3" s="141"/>
+      <c r="X3" s="142"/>
+      <c r="Y3" s="142"/>
+      <c r="Z3" s="142"/>
+      <c r="AA3" s="143"/>
+      <c r="AB3" s="122"/>
+      <c r="AC3" s="123"/>
+      <c r="AD3" s="123"/>
+      <c r="AE3" s="123"/>
+      <c r="AF3" s="123"/>
+      <c r="AG3" s="123"/>
+      <c r="AH3" s="124"/>
+      <c r="AI3" s="122"/>
+      <c r="AJ3" s="123"/>
+      <c r="AK3" s="123"/>
+      <c r="AL3" s="123"/>
+      <c r="AM3" s="123"/>
+      <c r="AN3" s="123"/>
+      <c r="AO3" s="124"/>
+      <c r="AP3" s="114"/>
       <c r="AQ3" s="19" t="s">
         <v>38</v>
       </c>
       <c r="AR3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AS3" s="111" t="s">
+      <c r="AS3" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="AT3" s="111"/>
-      <c r="AU3" s="151" t="s">
+      <c r="AT3" s="115"/>
+      <c r="AU3" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="AV3" s="151"/>
-      <c r="AW3" s="111"/>
-      <c r="AX3" s="111"/>
-      <c r="AY3" s="111"/>
-      <c r="AZ3" s="111"/>
-      <c r="BA3" s="111"/>
-      <c r="BB3" s="111"/>
-      <c r="BC3" s="111"/>
-      <c r="BD3" s="111"/>
-      <c r="BE3" s="111"/>
-      <c r="BF3" s="111"/>
-      <c r="BG3" s="111"/>
-      <c r="BH3" s="111"/>
-      <c r="BI3" s="111"/>
-      <c r="BJ3" s="111"/>
-      <c r="BK3" s="111"/>
-      <c r="BL3" s="111"/>
-      <c r="BM3" s="111"/>
-      <c r="BN3" s="111"/>
-      <c r="BO3" s="111"/>
-      <c r="BP3" s="111"/>
-      <c r="BQ3" s="111"/>
-      <c r="BR3" s="111"/>
-      <c r="BS3" s="111"/>
-      <c r="BT3" s="111"/>
-      <c r="BU3" s="111"/>
-      <c r="BV3" s="111"/>
-      <c r="BW3" s="112"/>
-      <c r="BX3" s="111"/>
-      <c r="BY3" s="111"/>
-      <c r="BZ3" s="112"/>
-      <c r="CA3" s="111"/>
-      <c r="CB3" s="111"/>
-      <c r="CC3" s="112"/>
-      <c r="CD3" s="149"/>
-      <c r="CE3" s="109"/>
-      <c r="CF3" s="110"/>
+      <c r="AV3" s="116"/>
+      <c r="AW3" s="115"/>
+      <c r="AX3" s="115"/>
+      <c r="AY3" s="115"/>
+      <c r="AZ3" s="115"/>
+      <c r="BA3" s="115"/>
+      <c r="BB3" s="115"/>
+      <c r="BC3" s="115"/>
+      <c r="BD3" s="115"/>
+      <c r="BE3" s="115"/>
+      <c r="BF3" s="115"/>
+      <c r="BG3" s="115"/>
+      <c r="BH3" s="115"/>
+      <c r="BI3" s="115"/>
+      <c r="BJ3" s="115"/>
+      <c r="BK3" s="115"/>
+      <c r="BL3" s="115"/>
+      <c r="BM3" s="115"/>
+      <c r="BN3" s="115"/>
+      <c r="BO3" s="115"/>
+      <c r="BP3" s="115"/>
+      <c r="BQ3" s="115"/>
+      <c r="BR3" s="115"/>
+      <c r="BS3" s="115"/>
+      <c r="BT3" s="115"/>
+      <c r="BU3" s="115"/>
+      <c r="BV3" s="115"/>
+      <c r="BW3" s="125"/>
+      <c r="BX3" s="115"/>
+      <c r="BY3" s="115"/>
+      <c r="BZ3" s="125"/>
+      <c r="CA3" s="115"/>
+      <c r="CB3" s="115"/>
+      <c r="CC3" s="125"/>
+      <c r="CD3" s="113"/>
+      <c r="CE3" s="148"/>
+      <c r="CF3" s="149"/>
     </row>
     <row r="4" spans="1:84" ht="45">
-      <c r="A4" s="147"/>
-      <c r="B4" s="147"/>
-      <c r="C4" s="153"/>
+      <c r="A4" s="111"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="118"/>
       <c r="D4" s="8" t="s">
         <v>8</v>
       </c>
@@ -5585,7 +5585,7 @@
       <c r="H4" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="I4" s="132"/>
+      <c r="I4" s="135"/>
       <c r="J4" s="2" t="s">
         <v>71</v>
       </c>
@@ -5613,10 +5613,10 @@
       <c r="R4" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="S4" s="133"/>
-      <c r="T4" s="133"/>
-      <c r="U4" s="133"/>
-      <c r="V4" s="134"/>
+      <c r="S4" s="136"/>
+      <c r="T4" s="136"/>
+      <c r="U4" s="136"/>
+      <c r="V4" s="137"/>
       <c r="W4" s="10" t="s">
         <v>5</v>
       </c>
@@ -13481,6 +13481,24 @@
   </sheetData>
   <autoFilter ref="A5:CF35"/>
   <mergeCells count="34">
+    <mergeCell ref="CE1:CF3"/>
+    <mergeCell ref="BU2:BW3"/>
+    <mergeCell ref="AI1:AO3"/>
+    <mergeCell ref="CA2:CC3"/>
+    <mergeCell ref="AP1:CC1"/>
+    <mergeCell ref="AB1:AH3"/>
+    <mergeCell ref="BX2:BZ3"/>
+    <mergeCell ref="D1:H3"/>
+    <mergeCell ref="I1:V2"/>
+    <mergeCell ref="W1:AA3"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="T3:T4"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="CD1:CD3"/>
     <mergeCell ref="AP2:AP3"/>
@@ -13497,24 +13515,6 @@
     <mergeCell ref="BR2:BT3"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:C4"/>
-    <mergeCell ref="AB1:AH3"/>
-    <mergeCell ref="BX2:BZ3"/>
-    <mergeCell ref="D1:H3"/>
-    <mergeCell ref="I1:V2"/>
-    <mergeCell ref="W1:AA3"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="CE1:CF3"/>
-    <mergeCell ref="BU2:BW3"/>
-    <mergeCell ref="AI1:AO3"/>
-    <mergeCell ref="CA2:CC3"/>
-    <mergeCell ref="AP1:CC1"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6">

</xml_diff>